<commit_message>
Final Lock: Pivot logic successful, ROIC calculated, and visuals generated
</commit_message>
<xml_diff>
--- a/data/Executive_Performance_Summary.xlsx
+++ b/data/Executive_Performance_Summary.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,27 +436,27 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Entity</t>
+          <t>entity</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Revenue</t>
+          <t>revenue</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>NOPAT</t>
+          <t>assets</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Assets</t>
+          <t>nopat</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>ROIC_%</t>
+          <t>roic_%</t>
         </is>
       </c>
     </row>
@@ -470,101 +470,84 @@
         <v>423000</v>
       </c>
       <c r="C2" t="n">
+        <v>189000</v>
+      </c>
+      <c r="D2" t="n">
         <v>317250</v>
       </c>
-      <c r="D2" t="n">
-        <v>189000</v>
-      </c>
       <c r="E2" t="n">
-        <v>167.8571428571429</v>
+        <v>167.86</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Terra-Grid</t>
+          <t>FinShield Re</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>5270500</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>2100000</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
+        <v>3952875</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>BioGrowth</t>
+          <t>Nexus Strategic</t>
         </is>
       </c>
       <c r="B4" t="n">
+        <v>869200</v>
+      </c>
+      <c r="C4" t="n">
         <v>0</v>
       </c>
-      <c r="C4" t="n">
-        <v>-446925</v>
-      </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>651900</v>
       </c>
       <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>FinShield Re</t>
+          <t>Omni-Retail</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5270500</v>
+        <v>9483000</v>
       </c>
       <c r="C5" t="n">
-        <v>3952875</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>7112250</v>
       </c>
       <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>Nexus Strategic</t>
+          <t>Terra-Grid</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>869200</v>
+        <v>0</v>
       </c>
       <c r="C6" t="n">
-        <v>294150</v>
+        <v>2100000</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
-      <c r="E6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Omni-Retail</t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>9483000</v>
-      </c>
-      <c r="C7" t="n">
-        <v>7112250</v>
-      </c>
-      <c r="D7" t="n">
+      <c r="E6" t="n">
         <v>0</v>
       </c>
-      <c r="E7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>